<commit_message>
new cases, supplemented table
</commit_message>
<xml_diff>
--- a/Tests_app3.xlsx
+++ b/Tests_app3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\REYAR\statsomat\Tests\Confirmatory-factor-analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berit\Documents\GitHub\Confirmatory-factor-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B863ACD-D627-4CFB-BE82-EC5BFB4C3711}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA1BD8A-9EE7-4919-806A-25FA739990F9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{740F734F-E3CE-4708-97FD-7DA20DC01FA8}"/>
+    <workbookView xWindow="-28920" yWindow="-3780" windowWidth="29040" windowHeight="15840" xr2:uid="{740F734F-E3CE-4708-97FD-7DA20DC01FA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="150">
   <si>
     <t>Basic Information</t>
   </si>
@@ -582,6 +582,54 @@
   </si>
   <si>
     <t>Errors in R Code 14/01/2021</t>
+  </si>
+  <si>
+    <t>auto-auto</t>
+  </si>
+  <si>
+    <t>UTF8-auto</t>
+  </si>
+  <si>
+    <t>UTF8-dot</t>
+  </si>
+  <si>
+    <t>UTF8-dot: no r-code</t>
+  </si>
+  <si>
+    <t>auto-auto: no R-Code</t>
+  </si>
+  <si>
+    <t>auto-comma: no rcode, seems like the comma-seperation goes wrong (for comma and dot)</t>
+  </si>
+  <si>
+    <t>auto-dot: no rcode (Error: Improper CFA solution. This can be due to: Outliers, small sample size,
+multicollinearity, model misspecification etc.)</t>
+  </si>
+  <si>
+    <t>auto-auto: no rcode: Error: Improper CFA solution. This can be due to: Outliers, small sample size,
+multicollinearity, model misspecification etc.</t>
+  </si>
+  <si>
+    <t>utf8-dot</t>
+  </si>
+  <si>
+    <t>utf8-auto</t>
+  </si>
+  <si>
+    <t>auto-dot</t>
+  </si>
+  <si>
+    <t>auto-auto: Error: Improper CFA solution. This can be due to: Outliers, small sample size, multicollinearity, model misspecification etc.</t>
+  </si>
+  <si>
+    <t>Higher-order factors were ignored.</t>
+  </si>
+  <si>
+    <t>discriminant validity</t>
+  </si>
+  <si>
+    <t>UTF8-comma:No rcode, Error: Improper CFA solution. This can be due to: Outliers, small sample size,
+multicollinearity, model misspecification etc.</t>
   </si>
 </sst>
 </file>
@@ -1183,7 +1231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1324,9 +1372,99 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1336,101 +1474,26 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1746,148 +1809,153 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AE19831-7C20-4D34-AF7C-EEDA5511FDD6}">
-  <dimension ref="A1:S37"/>
+  <dimension ref="A1:T37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="L5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="T5" sqref="T5"/>
+      <selection pane="bottomRight" activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="8.1328125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="14.86328125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="17.3984375" style="5" customWidth="1"/>
     <col min="4" max="4" width="13" style="5" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" style="5" customWidth="1"/>
-    <col min="12" max="12" width="19.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="22.59765625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="18.265625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="17.59765625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="20.3984375" style="5" customWidth="1"/>
+    <col min="9" max="9" width="22.265625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="16.265625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="17.265625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="19.59765625" style="5" customWidth="1"/>
     <col min="13" max="13" width="25" style="2" customWidth="1"/>
-    <col min="14" max="14" width="17.5703125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="23.140625" style="2" customWidth="1"/>
-    <col min="16" max="16" width="22.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="17.59765625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="23.1328125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="22.1328125" style="2" customWidth="1"/>
     <col min="17" max="17" width="26" style="5" customWidth="1"/>
-    <col min="18" max="18" width="32.85546875" style="5" customWidth="1"/>
-    <col min="19" max="19" width="18.85546875" style="2" customWidth="1"/>
-    <col min="20" max="20" width="18.5703125" style="2" customWidth="1"/>
-    <col min="21" max="16384" width="11.42578125" style="2"/>
+    <col min="18" max="18" width="32.86328125" style="5" customWidth="1"/>
+    <col min="19" max="19" width="18.86328125" style="5" customWidth="1"/>
+    <col min="20" max="20" width="18.59765625" style="2" customWidth="1"/>
+    <col min="21" max="16384" width="11.3984375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="54" t="s">
+    <row r="1" spans="1:20" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="81" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="64" t="s">
+      <c r="E1" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="67" t="s">
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="50" t="s">
+      <c r="M1" s="65"/>
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="56" t="s">
         <v>119</v>
       </c>
-      <c r="R1" s="50" t="s">
+      <c r="R1" s="56" t="s">
         <v>128</v>
       </c>
-      <c r="S1" s="50" t="s">
+      <c r="S1" s="56" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="55"/>
-      <c r="B2" s="58"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="70" t="s">
+      <c r="T1" s="88" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="51"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="67" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="84" t="s">
         <v>26</v>
       </c>
       <c r="G2" s="85"/>
-      <c r="H2" s="72" t="s">
+      <c r="H2" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="72" t="s">
+      <c r="I2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="72" t="s">
+      <c r="J2" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="74" t="s">
+      <c r="K2" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="82" t="s">
+      <c r="L2" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="76" t="s">
+      <c r="M2" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="76" t="s">
+      <c r="N2" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="78" t="s">
+      <c r="O2" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="80" t="s">
+      <c r="P2" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="50"/>
-      <c r="R2" s="50"/>
-      <c r="S2" s="50"/>
-    </row>
-    <row r="3" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="56"/>
-      <c r="B3" s="59"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="71"/>
+      <c r="Q2" s="56"/>
+      <c r="R2" s="56"/>
+      <c r="S2" s="56"/>
+      <c r="T2" s="88"/>
+    </row>
+    <row r="3" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="52"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="68"/>
       <c r="F3" s="40" t="s">
         <v>31</v>
       </c>
       <c r="G3" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="75"/>
-      <c r="L3" s="83"/>
-      <c r="M3" s="77"/>
-      <c r="N3" s="77"/>
-      <c r="O3" s="79"/>
-      <c r="P3" s="81"/>
-      <c r="Q3" s="50"/>
-      <c r="R3" s="50"/>
-      <c r="S3" s="50"/>
-    </row>
-    <row r="4" spans="1:19" s="11" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="80"/>
+      <c r="M3" s="74"/>
+      <c r="N3" s="74"/>
+      <c r="O3" s="76"/>
+      <c r="P3" s="78"/>
+      <c r="Q3" s="56"/>
+      <c r="R3" s="56"/>
+      <c r="S3" s="56"/>
+      <c r="T3" s="88"/>
+    </row>
+    <row r="4" spans="1:20" s="11" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="48"/>
       <c r="B4" s="17"/>
       <c r="C4" s="18" t="s">
@@ -1932,12 +2000,13 @@
       <c r="P4" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="Q4" s="50"/>
-      <c r="R4" s="50"/>
-      <c r="S4" s="50"/>
-    </row>
-    <row r="5" spans="1:19" ht="123.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="60" t="s">
+      <c r="Q4" s="56"/>
+      <c r="R4" s="56"/>
+      <c r="S4" s="56"/>
+      <c r="T4" s="88"/>
+    </row>
+    <row r="5" spans="1:20" ht="123.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="57" t="s">
         <v>43</v>
       </c>
       <c r="B5" s="19" t="s">
@@ -1981,9 +2050,13 @@
       <c r="R5" s="46" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="61"/>
+      <c r="S5" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="T5" s="91"/>
+    </row>
+    <row r="6" spans="1:20" ht="56.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="58"/>
       <c r="B6" s="20" t="s">
         <v>11</v>
       </c>
@@ -2029,9 +2102,15 @@
       <c r="R6" s="47" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" ht="96.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="61"/>
+      <c r="S6" s="47" t="s">
+        <v>139</v>
+      </c>
+      <c r="T6" s="89" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="96.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="58"/>
       <c r="B7" s="20" t="s">
         <v>12</v>
       </c>
@@ -2075,9 +2154,13 @@
       </c>
       <c r="Q7" s="41"/>
       <c r="R7" s="41"/>
-    </row>
-    <row r="8" spans="1:19" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="61"/>
+      <c r="S7" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="T7" s="91"/>
+    </row>
+    <row r="8" spans="1:20" ht="71.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="58"/>
       <c r="B8" s="20" t="s">
         <v>14</v>
       </c>
@@ -2114,10 +2197,10 @@
       <c r="M8" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="N8" s="62" t="s">
+      <c r="N8" s="59" t="s">
         <v>62</v>
       </c>
-      <c r="O8" s="63"/>
+      <c r="O8" s="60"/>
       <c r="P8" s="28" t="s">
         <v>60</v>
       </c>
@@ -2125,9 +2208,13 @@
       <c r="R8" s="43" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="61"/>
+      <c r="S8" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="T8" s="91"/>
+    </row>
+    <row r="9" spans="1:20" ht="62.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="58"/>
       <c r="B9" s="20" t="s">
         <v>15</v>
       </c>
@@ -2167,9 +2254,13 @@
       </c>
       <c r="Q9" s="42"/>
       <c r="R9" s="41"/>
-    </row>
-    <row r="10" spans="1:19" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="61"/>
+      <c r="S9" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="T9" s="91"/>
+    </row>
+    <row r="10" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="58"/>
       <c r="B10" s="20" t="s">
         <v>16</v>
       </c>
@@ -2209,9 +2300,15 @@
       <c r="R10" s="43" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" ht="63.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="61"/>
+      <c r="S10" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="T10" s="89" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="63.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="58"/>
       <c r="B11" s="20" t="s">
         <v>74</v>
       </c>
@@ -2253,9 +2350,13 @@
       </c>
       <c r="Q11" s="41"/>
       <c r="R11" s="41"/>
-    </row>
-    <row r="12" spans="1:19" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="61"/>
+      <c r="S11" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="T11" s="91"/>
+    </row>
+    <row r="12" spans="1:20" ht="64.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="58"/>
       <c r="B12" s="20" t="s">
         <v>75</v>
       </c>
@@ -2303,9 +2404,13 @@
       <c r="R12" s="47" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="61"/>
+      <c r="S12" s="47" t="s">
+        <v>138</v>
+      </c>
+      <c r="T12" s="89"/>
+    </row>
+    <row r="13" spans="1:20" ht="50.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="58"/>
       <c r="B13" s="20" t="s">
         <v>80</v>
       </c>
@@ -2349,9 +2454,13 @@
       <c r="R13" s="47" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="61"/>
+      <c r="S13" s="47" t="s">
+        <v>140</v>
+      </c>
+      <c r="T13" s="89"/>
+    </row>
+    <row r="14" spans="1:20" ht="53.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="58"/>
       <c r="B14" s="20" t="s">
         <v>88</v>
       </c>
@@ -2397,9 +2506,11 @@
       <c r="R14" s="47" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" s="23" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="61"/>
+      <c r="S14" s="42"/>
+      <c r="T14" s="89"/>
+    </row>
+    <row r="15" spans="1:20" s="23" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="58"/>
       <c r="B15" s="22" t="s">
         <v>91</v>
       </c>
@@ -2443,9 +2554,11 @@
       <c r="R15" s="47" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="61"/>
+      <c r="S15" s="86"/>
+      <c r="T15" s="90"/>
+    </row>
+    <row r="16" spans="1:20" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="58"/>
       <c r="B16" s="20" t="s">
         <v>89</v>
       </c>
@@ -2493,9 +2606,11 @@
       <c r="R16" s="47" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="61"/>
+      <c r="S16" s="42"/>
+      <c r="T16" s="89"/>
+    </row>
+    <row r="17" spans="1:20" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="58"/>
       <c r="B17" s="20" t="s">
         <v>102</v>
       </c>
@@ -2519,9 +2634,11 @@
       <c r="R17" s="47" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" ht="55.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="61"/>
+      <c r="S17" s="42"/>
+      <c r="T17" s="89"/>
+    </row>
+    <row r="18" spans="1:20" ht="55.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="58"/>
       <c r="B18" s="20" t="s">
         <v>103</v>
       </c>
@@ -2547,9 +2664,11 @@
       <c r="R18" s="47" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="61"/>
+      <c r="S18" s="42"/>
+      <c r="T18" s="89"/>
+    </row>
+    <row r="19" spans="1:20" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="58"/>
       <c r="B19" s="20" t="s">
         <v>93</v>
       </c>
@@ -2595,9 +2714,11 @@
       <c r="R19" s="47" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="61"/>
+      <c r="S19" s="42"/>
+      <c r="T19" s="89"/>
+    </row>
+    <row r="20" spans="1:20" ht="54.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="58"/>
       <c r="B20" s="20" t="s">
         <v>95</v>
       </c>
@@ -2643,9 +2764,13 @@
       <c r="R20" s="43" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" ht="54.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="61"/>
+      <c r="S20" s="43" t="s">
+        <v>141</v>
+      </c>
+      <c r="T20" s="89"/>
+    </row>
+    <row r="21" spans="1:20" ht="54.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="58"/>
       <c r="B21" s="25" t="s">
         <v>104</v>
       </c>
@@ -2691,9 +2816,11 @@
       <c r="R21" s="47" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" ht="58.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="61"/>
+      <c r="S21" s="42"/>
+      <c r="T21" s="89"/>
+    </row>
+    <row r="22" spans="1:20" ht="58.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="58"/>
       <c r="B22" s="25" t="s">
         <v>107</v>
       </c>
@@ -2735,9 +2862,15 @@
       </c>
       <c r="Q22" s="41"/>
       <c r="R22" s="41"/>
-    </row>
-    <row r="23" spans="1:18" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="61"/>
+      <c r="S22" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="T22" s="92" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" ht="43.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="58"/>
       <c r="B23" s="25" t="s">
         <v>109</v>
       </c>
@@ -2783,9 +2916,15 @@
       <c r="R23" s="43" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" ht="53.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="61"/>
+      <c r="S23" s="43" t="s">
+        <v>142</v>
+      </c>
+      <c r="T23" s="89" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" ht="53.65" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="58"/>
       <c r="B24" s="25" t="s">
         <v>112</v>
       </c>
@@ -2829,9 +2968,13 @@
       </c>
       <c r="Q24" s="41"/>
       <c r="R24" s="41"/>
-    </row>
-    <row r="25" spans="1:18" ht="54.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="61"/>
+      <c r="S24" s="41" t="s">
+        <v>143</v>
+      </c>
+      <c r="T24" s="91"/>
+    </row>
+    <row r="25" spans="1:20" ht="54.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="58"/>
       <c r="B25" s="25" t="s">
         <v>113</v>
       </c>
@@ -2877,9 +3020,13 @@
       </c>
       <c r="Q25" s="41"/>
       <c r="R25" s="41"/>
-    </row>
-    <row r="26" spans="1:18" ht="52.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="61"/>
+      <c r="S25" s="41" t="s">
+        <v>144</v>
+      </c>
+      <c r="T25" s="91"/>
+    </row>
+    <row r="26" spans="1:20" ht="52.35" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="58"/>
       <c r="B26" s="25" t="s">
         <v>118</v>
       </c>
@@ -2925,9 +3072,15 @@
       </c>
       <c r="Q26" s="41"/>
       <c r="R26" s="41"/>
-    </row>
-    <row r="27" spans="1:18" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="61"/>
+      <c r="S26" s="41" t="s">
+        <v>145</v>
+      </c>
+      <c r="T26" s="89" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" ht="48.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="58"/>
       <c r="B27" s="25" t="s">
         <v>120</v>
       </c>
@@ -2953,9 +3106,15 @@
       <c r="R27" s="43" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" ht="50.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="61"/>
+      <c r="S27" s="87" t="s">
+        <v>146</v>
+      </c>
+      <c r="T27" s="89" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" ht="50.65" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="58"/>
       <c r="B28" s="32" t="s">
         <v>121</v>
       </c>
@@ -2999,9 +3158,13 @@
       </c>
       <c r="Q28" s="45"/>
       <c r="R28" s="41"/>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A29" s="61"/>
+      <c r="S28" s="47" t="s">
+        <v>147</v>
+      </c>
+      <c r="T28" s="91"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A29" s="58"/>
       <c r="B29" s="37"/>
       <c r="C29" s="38"/>
       <c r="D29" s="38"/>
@@ -3019,8 +3182,8 @@
       <c r="P29" s="39"/>
       <c r="Q29" s="39"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A30" s="61"/>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A30" s="58"/>
       <c r="B30" s="37"/>
       <c r="C30" s="38"/>
       <c r="D30" s="38"/>
@@ -3038,8 +3201,8 @@
       <c r="P30" s="39"/>
       <c r="Q30" s="39"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A31" s="61"/>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A31" s="58"/>
       <c r="B31" s="37"/>
       <c r="C31" s="38"/>
       <c r="D31" s="38"/>
@@ -3057,8 +3220,8 @@
       <c r="P31" s="39"/>
       <c r="Q31" s="39"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A32" s="61"/>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A32" s="58"/>
       <c r="B32" s="37"/>
       <c r="C32" s="38"/>
       <c r="D32" s="38"/>
@@ -3076,7 +3239,7 @@
       <c r="P32" s="39"/>
       <c r="Q32" s="39"/>
     </row>
-    <row r="33" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -3092,7 +3255,7 @@
       <c r="O33" s="5"/>
       <c r="P33" s="5"/>
     </row>
-    <row r="34" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -3108,7 +3271,7 @@
       <c r="O34" s="5"/>
       <c r="P34" s="5"/>
     </row>
-    <row r="35" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -3124,7 +3287,7 @@
       <c r="O35" s="5"/>
       <c r="P35" s="5"/>
     </row>
-    <row r="36" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -3140,14 +3303,21 @@
       <c r="O36" s="5"/>
       <c r="P36" s="5"/>
     </row>
-    <row r="37" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:16" x14ac:dyDescent="0.4">
       <c r="M37" s="5"/>
       <c r="N37" s="5"/>
       <c r="O37" s="5"/>
       <c r="P37" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="23">
+    <mergeCell ref="T1:T4"/>
+    <mergeCell ref="S1:S4"/>
+    <mergeCell ref="Q1:Q4"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="F2:G2"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="R1:R4"/>
@@ -3164,12 +3334,6 @@
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="P2:P3"/>
     <mergeCell ref="L2:L3"/>
-    <mergeCell ref="S1:S4"/>
-    <mergeCell ref="Q1:Q4"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="F2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
new cases, updated table
</commit_message>
<xml_diff>
--- a/Tests_app3.xlsx
+++ b/Tests_app3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\REYAR\statsomat\Tests\Confirmatory-factor-analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berit\Documents\GitHub\Confirmatory-factor-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254211B7-F1E7-41DD-AD60-A28122E73AC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2162FB43-6C1B-44C2-AAE9-20BB442EBB69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{740F734F-E3CE-4708-97FD-7DA20DC01FA8}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{740F734F-E3CE-4708-97FD-7DA20DC01FA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="152">
   <si>
     <t>Basic Information</t>
   </si>
@@ -591,6 +591,48 @@
   </si>
   <si>
     <t>higher-order error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unstandardized coefficient was fixed to 1 </t>
+  </si>
+  <si>
+    <t>because the standardized pattern coefficient of Hand Movements is at least moderate, it is possible that this task may measur both factors</t>
+  </si>
+  <si>
+    <t>"model fails both the exact-fit and close-fit tests and the lower bound of RMSEA's 90% confidence interval"</t>
+  </si>
+  <si>
+    <t>in source: "poor global fit";  in report: gof of the model is uncertain</t>
+  </si>
+  <si>
+    <t>in source: "hand movement measures both factors is plausible"; in report: no significant and relevant modification indices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Information about the model </t>
+  </si>
+  <si>
+    <t>all values of approximate-fit indexes are generally favorable</t>
+  </si>
+  <si>
+    <t>"few apparent problems", no absolute correlation residuals exceeded .10</t>
+  </si>
+  <si>
+    <t>The model just passes the exact-fit test at the .05 level; it also passes the close-fit test  at the same level. Values of the CFI and SRMR are generally favorable, but results on  the RMSEA are poor:</t>
+  </si>
+  <si>
+    <t>Based on all these results, the respecified nonrecursive model with a direct effect from  continuance organizational commitment to occupational turnover intention is retained</t>
+  </si>
+  <si>
+    <t>the impact of the intention to leave one’s place of work on the  intention to leave one’s profession is greater than the magnitude of the influence in  the other direction by a ratio of almost eight</t>
+  </si>
+  <si>
+    <t>Error: Improper CFA solution. This can be due to: Outliers, small sample size, multicollinearity, model misspecification etc.</t>
+  </si>
+  <si>
+    <t>Case25-one factor model</t>
+  </si>
+  <si>
+    <t>poor model fit- not useful</t>
   </si>
 </sst>
 </file>
@@ -648,7 +690,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -681,12 +723,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -710,7 +746,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -1194,11 +1230,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1223,7 +1270,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1236,10 +1283,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1248,29 +1295,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1300,19 +1344,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1325,24 +1369,100 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1357,103 +1477,29 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1770,142 +1816,142 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AE19831-7C20-4D34-AF7C-EEDA5511FDD6}">
-  <dimension ref="A1:R38"/>
+  <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="L23" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="U29" sqref="U29"/>
+      <selection pane="bottomRight" activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="8.1328125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="14.86328125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="17.3984375" style="5" customWidth="1"/>
     <col min="4" max="4" width="13" style="5" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" style="5" customWidth="1"/>
-    <col min="12" max="12" width="19.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="22.59765625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="18.265625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="17.59765625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="20.3984375" style="5" customWidth="1"/>
+    <col min="9" max="9" width="22.265625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="16.265625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="17.265625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="19.59765625" style="5" customWidth="1"/>
     <col min="13" max="13" width="25" style="2" customWidth="1"/>
-    <col min="14" max="14" width="17.5703125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="23.140625" style="2" customWidth="1"/>
-    <col min="16" max="16" width="22.140625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="34.28515625" style="5" customWidth="1"/>
-    <col min="18" max="18" width="18.5703125" style="2" customWidth="1"/>
-    <col min="19" max="16384" width="11.42578125" style="2"/>
+    <col min="14" max="14" width="17.59765625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="23.1328125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="22.1328125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="34.265625" style="5" customWidth="1"/>
+    <col min="18" max="18" width="18.59765625" style="2" customWidth="1"/>
+    <col min="19" max="16384" width="11.3984375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="62" t="s">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="55" t="s">
+      <c r="D1" s="78" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="72" t="s">
+      <c r="E1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="75" t="s">
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="76"/>
-      <c r="P1" s="77"/>
-      <c r="Q1" s="54" t="s">
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="77" t="s">
         <v>122</v>
       </c>
-      <c r="R1" s="53" t="s">
+      <c r="R1" s="76" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="63"/>
-      <c r="B2" s="66"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="78" t="s">
+    <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="47"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="60" t="s">
+      <c r="F2" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="61"/>
-      <c r="H2" s="80" t="s">
+      <c r="G2" s="82"/>
+      <c r="H2" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="80" t="s">
+      <c r="I2" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="80" t="s">
+      <c r="J2" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="82" t="s">
+      <c r="K2" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="88" t="s">
+      <c r="L2" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="58" t="s">
+      <c r="M2" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="N2" s="58" t="s">
+      <c r="N2" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="84" t="s">
+      <c r="O2" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="86" t="s">
+      <c r="P2" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="53"/>
-    </row>
-    <row r="3" spans="1:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="64"/>
-      <c r="B3" s="67"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="37" t="s">
+      <c r="Q2" s="77"/>
+      <c r="R2" s="76"/>
+    </row>
+    <row r="3" spans="1:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="48"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="37" t="s">
+      <c r="G3" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="83"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="59"/>
-      <c r="N3" s="59"/>
-      <c r="O3" s="85"/>
-      <c r="P3" s="87"/>
-      <c r="Q3" s="54"/>
-      <c r="R3" s="53"/>
-    </row>
-    <row r="4" spans="1:18" s="10" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="67"/>
+      <c r="L3" s="75"/>
+      <c r="M3" s="69"/>
+      <c r="N3" s="69"/>
+      <c r="O3" s="71"/>
+      <c r="P3" s="73"/>
+      <c r="Q3" s="77"/>
+      <c r="R3" s="76"/>
+    </row>
+    <row r="4" spans="1:18" s="10" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="38"/>
       <c r="B4" s="15"/>
       <c r="C4" s="16" t="s">
         <v>7</v>
@@ -1949,11 +1995,11 @@
       <c r="P4" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="Q4" s="54"/>
-      <c r="R4" s="53"/>
-    </row>
-    <row r="5" spans="1:18" ht="123.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="68" t="s">
+      <c r="Q4" s="77"/>
+      <c r="R4" s="76"/>
+    </row>
+    <row r="5" spans="1:18" ht="123.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="52" t="s">
         <v>41</v>
       </c>
       <c r="B5" s="17" t="s">
@@ -1990,16 +2036,16 @@
       <c r="O5" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="P5" s="43" t="s">
+      <c r="P5" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="Q5" s="38" t="s">
+      <c r="Q5" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="R5" s="42"/>
-    </row>
-    <row r="6" spans="1:18" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="69"/>
+      <c r="R5" s="41"/>
+    </row>
+    <row r="6" spans="1:18" ht="56.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="53"/>
       <c r="B6" s="18" t="s">
         <v>11</v>
       </c>
@@ -2040,18 +2086,18 @@
       <c r="O6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="P6" s="27" t="s">
+      <c r="P6" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="Q6" s="41" t="s">
+      <c r="Q6" s="40" t="s">
         <v>131</v>
       </c>
-      <c r="R6" s="41" t="s">
+      <c r="R6" s="40" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="108" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="69"/>
+    <row r="7" spans="1:18" ht="108" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="53"/>
       <c r="B7" s="18" t="s">
         <v>12</v>
       </c>
@@ -2090,16 +2136,16 @@
       <c r="O7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="P7" s="28" t="s">
+      <c r="P7" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="Q7" s="38" t="s">
+      <c r="Q7" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="R7" s="42"/>
-    </row>
-    <row r="8" spans="1:18" ht="95.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="69"/>
+      <c r="R7" s="41"/>
+    </row>
+    <row r="8" spans="1:18" ht="95.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="53"/>
       <c r="B8" s="18" t="s">
         <v>14</v>
       </c>
@@ -2136,20 +2182,20 @@
       <c r="M8" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="N8" s="70" t="s">
+      <c r="N8" s="54" t="s">
         <v>130</v>
       </c>
-      <c r="O8" s="71"/>
-      <c r="P8" s="28" t="s">
+      <c r="O8" s="55"/>
+      <c r="P8" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="Q8" s="38" t="s">
+      <c r="Q8" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="R8" s="42"/>
-    </row>
-    <row r="9" spans="1:18" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="69"/>
+      <c r="R8" s="41"/>
+    </row>
+    <row r="9" spans="1:18" ht="62.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="53"/>
       <c r="B9" s="18" t="s">
         <v>15</v>
       </c>
@@ -2184,60 +2230,82 @@
       <c r="O9" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="P9" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q9" s="38" t="s">
+      <c r="P9" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q9" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="R9" s="42"/>
-    </row>
-    <row r="10" spans="1:18" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="69"/>
+      <c r="R9" s="41"/>
+    </row>
+    <row r="10" spans="1:18" ht="67.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="53"/>
       <c r="B10" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="44"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="44"/>
-      <c r="N10" s="44"/>
-      <c r="O10" s="44"/>
-      <c r="P10" s="45"/>
-      <c r="Q10" s="46"/>
-      <c r="R10" s="47"/>
-    </row>
-    <row r="11" spans="1:18" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="69"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="43"/>
+      <c r="O10" s="43"/>
+      <c r="P10" s="44"/>
+      <c r="Q10" s="37" t="s">
+        <v>123</v>
+      </c>
+      <c r="R10" s="41"/>
+    </row>
+    <row r="11" spans="1:18" ht="67.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="53"/>
       <c r="B11" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
-      <c r="N11" s="48"/>
-      <c r="O11" s="48"/>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="46"/>
-      <c r="R11" s="47"/>
-    </row>
-    <row r="12" spans="1:18" ht="63.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="69"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="E11" s="19"/>
+      <c r="F11" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="7"/>
+      <c r="H11" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="M11" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="O11" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="P11" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q11" s="37"/>
+      <c r="R11" s="41"/>
+    </row>
+    <row r="12" spans="1:18" ht="63.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="53"/>
       <c r="B12" s="18" t="s">
         <v>69</v>
       </c>
@@ -2274,16 +2342,16 @@
       <c r="O12" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="P12" s="28" t="s">
+      <c r="P12" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="Q12" s="38" t="s">
+      <c r="Q12" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="R12" s="42"/>
-    </row>
-    <row r="13" spans="1:18" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="69"/>
+      <c r="R12" s="41"/>
+    </row>
+    <row r="13" spans="1:18" ht="64.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="53"/>
       <c r="B13" s="18" t="s">
         <v>70</v>
       </c>
@@ -2324,18 +2392,18 @@
       <c r="O13" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="P13" s="45" t="s">
+      <c r="P13" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="Q13" s="41" t="s">
+      <c r="Q13" s="40" t="s">
         <v>131</v>
       </c>
-      <c r="R13" s="41" t="s">
+      <c r="R13" s="40" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="69"/>
+    <row r="14" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="53"/>
       <c r="B14" s="18" t="s">
         <v>75</v>
       </c>
@@ -2372,18 +2440,18 @@
       <c r="O14" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="P14" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q14" s="41" t="s">
+      <c r="P14" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q14" s="40" t="s">
         <v>131</v>
       </c>
-      <c r="R14" s="41" t="s">
+      <c r="R14" s="40" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="69"/>
+    <row r="15" spans="1:18" ht="53.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="53"/>
       <c r="B15" s="18" t="s">
         <v>83</v>
       </c>
@@ -2422,18 +2490,18 @@
       <c r="O15" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="P15" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q15" s="41" t="s">
+      <c r="P15" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q15" s="40" t="s">
         <v>131</v>
       </c>
-      <c r="R15" s="41" t="s">
+      <c r="R15" s="40" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="1:18" s="21" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="69"/>
+    <row r="16" spans="1:18" s="21" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="53"/>
       <c r="B16" s="20" t="s">
         <v>86</v>
       </c>
@@ -2470,18 +2538,18 @@
       <c r="O16" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="P16" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q16" s="41" t="s">
+      <c r="P16" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q16" s="40" t="s">
         <v>131</v>
       </c>
-      <c r="R16" s="41" t="s">
+      <c r="R16" s="40" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="69"/>
+    <row r="17" spans="1:19" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="53"/>
       <c r="B17" s="18" t="s">
         <v>84</v>
       </c>
@@ -2522,18 +2590,18 @@
       <c r="O17" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="P17" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q17" s="41" t="s">
+      <c r="P17" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q17" s="40" t="s">
         <v>131</v>
       </c>
-      <c r="R17" s="41" t="s">
+      <c r="R17" s="40" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="69"/>
+    <row r="18" spans="1:19" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="53"/>
       <c r="B18" s="18" t="s">
         <v>97</v>
       </c>
@@ -2552,16 +2620,16 @@
       <c r="M18" s="19"/>
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
-      <c r="P18" s="26"/>
-      <c r="Q18" s="41" t="s">
+      <c r="P18" s="25"/>
+      <c r="Q18" s="40" t="s">
         <v>131</v>
       </c>
-      <c r="R18" s="41" t="s">
+      <c r="R18" s="40" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="55.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="69"/>
+    <row r="19" spans="1:19" ht="55.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="53"/>
       <c r="B19" s="18" t="s">
         <v>98</v>
       </c>
@@ -2582,16 +2650,16 @@
       <c r="M19" s="6"/>
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
-      <c r="P19" s="26"/>
-      <c r="Q19" s="41" t="s">
+      <c r="P19" s="25"/>
+      <c r="Q19" s="40" t="s">
         <v>131</v>
       </c>
-      <c r="R19" s="41" t="s">
+      <c r="R19" s="40" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="69"/>
+    <row r="20" spans="1:19" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="53"/>
       <c r="B20" s="18" t="s">
         <v>88</v>
       </c>
@@ -2630,18 +2698,18 @@
       <c r="O20" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="P20" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q20" s="41" t="s">
+      <c r="P20" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q20" s="40" t="s">
         <v>131</v>
       </c>
-      <c r="R20" s="41" t="s">
+      <c r="R20" s="40" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="69"/>
+    <row r="21" spans="1:19" ht="54.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="53"/>
       <c r="B21" s="18" t="s">
         <v>90</v>
       </c>
@@ -2680,18 +2748,18 @@
       <c r="O21" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="P21" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q21" s="41" t="s">
+      <c r="P21" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q21" s="40" t="s">
         <v>136</v>
       </c>
-      <c r="R21" s="41" t="s">
+      <c r="R21" s="40" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="54.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="69"/>
+    <row r="22" spans="1:19" ht="54.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="53"/>
       <c r="B22" s="23" t="s">
         <v>99</v>
       </c>
@@ -2730,18 +2798,18 @@
       <c r="O22" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="P22" s="28" t="s">
+      <c r="P22" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="Q22" s="41" t="s">
+      <c r="Q22" s="40" t="s">
         <v>131</v>
       </c>
-      <c r="R22" s="41" t="s">
+      <c r="R22" s="40" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="58.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="69"/>
+    <row r="23" spans="1:19" ht="58.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="53"/>
       <c r="B23" s="23" t="s">
         <v>102</v>
       </c>
@@ -2778,16 +2846,16 @@
       <c r="O23" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="P23" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q23" s="38" t="s">
+      <c r="P23" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q23" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="R23" s="42"/>
-    </row>
-    <row r="24" spans="1:18" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="69"/>
+      <c r="R23" s="41"/>
+    </row>
+    <row r="24" spans="1:19" ht="43.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="53"/>
       <c r="B24" s="23" t="s">
         <v>104</v>
       </c>
@@ -2828,16 +2896,16 @@
       <c r="O24" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="P24" s="28"/>
-      <c r="Q24" s="41" t="s">
+      <c r="P24" s="27"/>
+      <c r="Q24" s="40" t="s">
         <v>136</v>
       </c>
-      <c r="R24" s="41" t="s">
+      <c r="R24" s="40" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="53.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="69"/>
+    <row r="25" spans="1:19" ht="53.65" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="53"/>
       <c r="B25" s="23" t="s">
         <v>107</v>
       </c>
@@ -2876,16 +2944,16 @@
       <c r="O25" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="P25" s="28" t="s">
+      <c r="P25" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="Q25" s="38" t="s">
+      <c r="Q25" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="R25" s="42"/>
-    </row>
-    <row r="26" spans="1:18" ht="54.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="69"/>
+      <c r="R25" s="41"/>
+    </row>
+    <row r="26" spans="1:19" ht="54.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="53"/>
       <c r="B26" s="23" t="s">
         <v>108</v>
       </c>
@@ -2926,16 +2994,16 @@
       <c r="O26" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="P26" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q26" s="38" t="s">
+      <c r="P26" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q26" s="37" t="s">
         <v>127</v>
       </c>
-      <c r="R26" s="42"/>
-    </row>
-    <row r="27" spans="1:18" ht="52.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="69"/>
+      <c r="R26" s="41"/>
+    </row>
+    <row r="27" spans="1:19" ht="52.35" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="53"/>
       <c r="B27" s="23" t="s">
         <v>113</v>
       </c>
@@ -2976,20 +3044,20 @@
       <c r="O27" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="P27" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q27" s="38" t="s">
+      <c r="P27" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q27" s="37" t="s">
         <v>128</v>
       </c>
-      <c r="R27" s="42"/>
-    </row>
-    <row r="28" spans="1:18" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="69"/>
+      <c r="R27" s="41"/>
+    </row>
+    <row r="28" spans="1:19" ht="48.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="53"/>
       <c r="B28" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="C28" s="40" t="s">
+      <c r="C28" s="39" t="s">
         <v>116</v>
       </c>
       <c r="D28" s="6"/>
@@ -3004,165 +3072,210 @@
       <c r="M28" s="6"/>
       <c r="N28" s="6"/>
       <c r="O28" s="6"/>
-      <c r="P28" s="26"/>
-      <c r="Q28" s="41" t="s">
+      <c r="P28" s="25"/>
+      <c r="Q28" s="40" t="s">
         <v>136</v>
       </c>
-      <c r="R28" s="41" t="s">
+      <c r="R28" s="40" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="50.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="69"/>
-      <c r="B29" s="29" t="s">
+    <row r="29" spans="1:19" ht="50.65" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="53"/>
+      <c r="B29" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="C29" s="30"/>
-      <c r="D29" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="E29" s="32" t="s">
+      <c r="C29" s="29"/>
+      <c r="D29" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="F29" s="30" t="s">
+      <c r="F29" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="G29" s="30"/>
-      <c r="H29" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="I29" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="J29" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="K29" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="L29" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="M29" s="30" t="s">
+      <c r="G29" s="29"/>
+      <c r="H29" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="I29" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="J29" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="K29" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="L29" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="M29" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="N29" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="O29" s="30" t="s">
+      <c r="N29" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="O29" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="P29" s="33" t="s">
+      <c r="P29" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="Q29" s="90" t="s">
+      <c r="Q29" s="83" t="s">
         <v>137</v>
       </c>
-      <c r="R29" s="90" t="s">
+      <c r="R29" s="83" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A30" s="69"/>
-      <c r="B30" s="34" t="s">
+    <row r="30" spans="1:19" ht="38.65" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="53"/>
+      <c r="B30" s="84" t="s">
         <v>133</v>
       </c>
-      <c r="C30" s="49"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="49"/>
-      <c r="G30" s="49"/>
-      <c r="H30" s="49"/>
-      <c r="I30" s="49"/>
-      <c r="J30" s="49"/>
-      <c r="K30" s="49"/>
-      <c r="L30" s="49"/>
-      <c r="M30" s="49"/>
-      <c r="N30" s="49"/>
-      <c r="O30" s="49"/>
-      <c r="P30" s="50"/>
-      <c r="Q30" s="51"/>
-      <c r="R30" s="52"/>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A31" s="69"/>
-      <c r="B31" s="34" t="s">
+      <c r="C30" s="85" t="s">
+        <v>143</v>
+      </c>
+      <c r="D30" s="86"/>
+      <c r="E30" s="86"/>
+      <c r="F30" s="86"/>
+      <c r="G30" s="86"/>
+      <c r="H30" s="86"/>
+      <c r="I30" s="86"/>
+      <c r="J30" s="86"/>
+      <c r="K30" s="86"/>
+      <c r="L30" s="86"/>
+      <c r="M30" s="86"/>
+      <c r="N30" s="86"/>
+      <c r="O30" s="86"/>
+      <c r="P30" s="87"/>
+      <c r="Q30" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="R30" s="88" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" ht="39.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="53"/>
+      <c r="B31" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="C31" s="49"/>
-      <c r="D31" s="49"/>
-      <c r="E31" s="49"/>
-      <c r="F31" s="49"/>
-      <c r="G31" s="49"/>
-      <c r="H31" s="49"/>
-      <c r="I31" s="49"/>
-      <c r="J31" s="49"/>
-      <c r="K31" s="49"/>
-      <c r="L31" s="49"/>
-      <c r="M31" s="49"/>
-      <c r="N31" s="49"/>
-      <c r="O31" s="50"/>
-      <c r="P31" s="50"/>
-      <c r="Q31" s="51"/>
-      <c r="R31" s="52"/>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A32" s="69"/>
-      <c r="B32" s="34" t="s">
+      <c r="C31" s="7"/>
+      <c r="D31" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" s="43"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="I31" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="J31" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="K31" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="L31" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="M31" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="N31" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="O31" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="P31" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q31" s="37"/>
+      <c r="R31" s="41"/>
+    </row>
+    <row r="32" spans="1:19" ht="39.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="53"/>
+      <c r="B32" s="84" t="s">
+        <v>150</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
+      <c r="O32" s="40"/>
+      <c r="P32" s="40"/>
+      <c r="Q32" s="40"/>
+      <c r="R32" s="88"/>
+      <c r="S32" s="21"/>
+    </row>
+    <row r="33" spans="1:18" ht="39.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="53"/>
+      <c r="B33" s="84" t="s">
         <v>135</v>
       </c>
-      <c r="C32" s="49"/>
-      <c r="D32" s="49"/>
-      <c r="E32" s="49"/>
-      <c r="F32" s="49"/>
-      <c r="G32" s="49"/>
-      <c r="H32" s="49"/>
-      <c r="I32" s="49"/>
-      <c r="J32" s="49"/>
-      <c r="K32" s="49"/>
-      <c r="L32" s="49"/>
-      <c r="M32" s="49"/>
-      <c r="N32" s="49"/>
-      <c r="O32" s="50"/>
-      <c r="P32" s="50"/>
-      <c r="Q32" s="51"/>
-      <c r="R32" s="52"/>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A33" s="69"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="35"/>
-      <c r="D33" s="35"/>
-      <c r="E33" s="35"/>
-      <c r="F33" s="35"/>
-      <c r="G33" s="35"/>
-      <c r="H33" s="35"/>
-      <c r="I33" s="35"/>
-      <c r="J33" s="35"/>
-      <c r="K33" s="35"/>
-      <c r="L33" s="35"/>
-      <c r="M33" s="35"/>
-      <c r="N33" s="35"/>
-      <c r="O33" s="36"/>
-      <c r="P33" s="36"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="5"/>
-      <c r="P34" s="5"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C33" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="M33" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="N33" s="19"/>
+      <c r="O33" s="40"/>
+      <c r="P33" s="40" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q33" s="89" t="s">
+        <v>136</v>
+      </c>
+      <c r="R33" s="88"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A34" s="53"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="34"/>
+      <c r="K34" s="34"/>
+      <c r="L34" s="34"/>
+      <c r="M34" s="34"/>
+      <c r="N34" s="34"/>
+      <c r="O34" s="35"/>
+      <c r="P34" s="35"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.4">
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -3178,7 +3291,7 @@
       <c r="O35" s="5"/>
       <c r="P35" s="5"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.4">
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -3194,7 +3307,7 @@
       <c r="O36" s="5"/>
       <c r="P36" s="5"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.4">
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -3210,17 +3323,40 @@
       <c r="O37" s="5"/>
       <c r="P37" s="5"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="M38" s="5"/>
-      <c r="N38" s="5"/>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
       <c r="O38" s="5"/>
       <c r="P38" s="5"/>
     </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="M39" s="5"/>
+      <c r="N39" s="5"/>
+      <c r="O39" s="5"/>
+      <c r="P39" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="22">
+    <mergeCell ref="C30:P30"/>
+    <mergeCell ref="R1:R4"/>
+    <mergeCell ref="Q1:Q4"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="F2:G2"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:B3"/>
-    <mergeCell ref="A5:A33"/>
+    <mergeCell ref="A5:A34"/>
     <mergeCell ref="N8:O8"/>
     <mergeCell ref="E1:K1"/>
     <mergeCell ref="L1:P1"/>
@@ -3233,12 +3369,6 @@
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="P2:P3"/>
     <mergeCell ref="L2:L3"/>
-    <mergeCell ref="R1:R4"/>
-    <mergeCell ref="Q1:Q4"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="F2:G2"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>